<commit_message>
Updates on the cat model
</commit_message>
<xml_diff>
--- a/models/14sectors_cat/land.xlsx
+++ b/models/14sectors_cat/land.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <definedName name="variation_primary_forests_area" localSheetId="1">Europe!$C$2</definedName>
     <definedName name="wood_energy_density" localSheetId="0">Global!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -256,7 +256,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Iñigo:
+          <t xml:space="preserve">Enric:
 </t>
         </r>
         <r>
@@ -267,8 +267,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">CAIT
-http://www.wri.org/resources/data-sets/cait-historical-emissions-data-countries-us-states-unfccc
+          <t xml:space="preserve">EDGAR
 </t>
         </r>
       </text>
@@ -1067,7 +1066,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="J48" sqref="I48:J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1183,8 +1182,8 @@
   </sheetPr>
   <dimension ref="A1:BN21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AB5" sqref="AB5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1988,81 +1987,107 @@
         <v>23</v>
       </c>
       <c r="C15" s="4">
-        <v>-0.29501957469948298</v>
+        <v>-0.34496931405827302</v>
       </c>
       <c r="D15" s="4">
-        <v>-0.29501419551768499</v>
+        <v>-0.46814242262519801</v>
       </c>
       <c r="E15" s="4">
-        <v>-0.285226655822994</v>
+        <v>-0.46609129011263106</v>
       </c>
       <c r="F15" s="4">
-        <v>-0.29510965510000098</v>
+        <v>-0.49515421907023205</v>
       </c>
       <c r="G15" s="4">
-        <v>-0.29510446800000001</v>
+        <v>-0.43664204247300598</v>
       </c>
       <c r="H15" s="4">
-        <v>-0.29509928569999999</v>
+        <v>-0.41879503143528102</v>
       </c>
       <c r="I15" s="4">
-        <v>-0.29509653949999998</v>
+        <v>-0.42498349624917697</v>
       </c>
       <c r="J15" s="4">
-        <v>-0.29520885149999798</v>
+        <v>-0.4181721856350456</v>
       </c>
       <c r="K15" s="4">
-        <v>-0.29503016589999997</v>
+        <v>-0.38851950639383398</v>
       </c>
       <c r="L15" s="4">
-        <v>-0.29519845569999997</v>
+        <v>-0.46841254940853805</v>
       </c>
       <c r="M15" s="4">
-        <v>-0.29508998359999999</v>
+        <v>-0.33033722222970902</v>
       </c>
       <c r="N15" s="4">
-        <v>-0.32775546849999998</v>
+        <v>-0.37792358760623901</v>
       </c>
       <c r="O15" s="4">
-        <v>-0.32771818409999998</v>
+        <v>-0.38759988127086309</v>
       </c>
       <c r="P15" s="4">
-        <v>-0.32725808360000003</v>
+        <v>-0.36132755199540101</v>
       </c>
       <c r="Q15" s="4">
-        <v>-0.32795720229999997</v>
+        <v>-0.37335515417665699</v>
       </c>
       <c r="R15" s="4">
-        <v>-0.32785511909999898</v>
+        <v>-0.31262835196880601</v>
       </c>
       <c r="S15" s="4">
-        <v>-0.342626737499999</v>
+        <v>-0.36857917375828403</v>
       </c>
       <c r="T15" s="4">
-        <v>-0.34198419730000101</v>
+        <v>-0.29009013615355</v>
       </c>
       <c r="U15" s="4">
-        <v>-0.342547157800001</v>
+        <v>-0.33518804786981399</v>
       </c>
       <c r="V15" s="4">
-        <v>-0.34320179969999998</v>
+        <v>-0.399988360089993</v>
       </c>
       <c r="W15" s="4">
-        <v>-0.34296992100000101</v>
+        <v>-0.31988691783600903</v>
       </c>
       <c r="X15" s="4">
-        <v>-0.42800970090000101</v>
+        <v>-0.31755958479959595</v>
       </c>
       <c r="Y15" s="4">
-        <v>-0.42809877999999901</v>
+        <v>-0.31369644998465401</v>
       </c>
       <c r="Z15" s="4">
-        <v>-0.42900656040000001</v>
+        <v>-0.296045027887887</v>
       </c>
       <c r="AA15" s="4">
-        <v>-0.42908028699999901</v>
-      </c>
-      <c r="AB15" s="4"/>
+        <v>-0.30862722177435603</v>
+      </c>
+      <c r="AB15" s="4">
+        <v>-0.309062138068257</v>
+      </c>
+      <c r="AC15">
+        <v>-0.29693685476449</v>
+      </c>
+      <c r="AD15">
+        <v>-0.27505925115152602</v>
+      </c>
+      <c r="AE15">
+        <v>-0.24473760610362399</v>
+      </c>
+      <c r="AF15">
+        <v>-0.24656475954628296</v>
+      </c>
+      <c r="AG15">
+        <v>-0.26476597050030798</v>
+      </c>
+      <c r="AH15">
+        <v>-0.22245570919959301</v>
+      </c>
+      <c r="AI15">
+        <v>-0.22419899523269299</v>
+      </c>
+      <c r="AJ15">
+        <v>-0.21516157963982299</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="9"/>
@@ -2098,7 +2123,7 @@
   </sheetPr>
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Correction of a bug in the model version compatibility
</commit_message>
<xml_diff>
--- a/models/14sectors_cat/land.xlsx
+++ b/models/14sectors_cat/land.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <definedName name="variation_primary_forests_area" localSheetId="1">Europe!$C$2</definedName>
     <definedName name="wood_energy_density" localSheetId="0">Global!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -256,7 +256,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Enric:
+          <t xml:space="preserve">Iñigo:
 </t>
         </r>
         <r>
@@ -267,7 +267,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">EDGAR
+          <t xml:space="preserve">CAIT
+http://www.wri.org/resources/data-sets/cait-historical-emissions-data-countries-us-states-unfccc
 </t>
         </r>
       </text>
@@ -1066,7 +1067,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J48" sqref="I48:J48"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1182,8 +1183,8 @@
   </sheetPr>
   <dimension ref="A1:BN21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AG15" sqref="AG15"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1987,107 +1988,81 @@
         <v>23</v>
       </c>
       <c r="C15" s="4">
-        <v>-0.34496931405827302</v>
+        <v>-0.29501957469948298</v>
       </c>
       <c r="D15" s="4">
-        <v>-0.46814242262519801</v>
+        <v>-0.29501419551768499</v>
       </c>
       <c r="E15" s="4">
-        <v>-0.46609129011263106</v>
+        <v>-0.285226655822994</v>
       </c>
       <c r="F15" s="4">
-        <v>-0.49515421907023205</v>
+        <v>-0.29510965510000098</v>
       </c>
       <c r="G15" s="4">
-        <v>-0.43664204247300598</v>
+        <v>-0.29510446800000001</v>
       </c>
       <c r="H15" s="4">
-        <v>-0.41879503143528102</v>
+        <v>-0.29509928569999999</v>
       </c>
       <c r="I15" s="4">
-        <v>-0.42498349624917697</v>
+        <v>-0.29509653949999998</v>
       </c>
       <c r="J15" s="4">
-        <v>-0.4181721856350456</v>
+        <v>-0.29520885149999798</v>
       </c>
       <c r="K15" s="4">
-        <v>-0.38851950639383398</v>
+        <v>-0.29503016589999997</v>
       </c>
       <c r="L15" s="4">
-        <v>-0.46841254940853805</v>
+        <v>-0.29519845569999997</v>
       </c>
       <c r="M15" s="4">
-        <v>-0.33033722222970902</v>
+        <v>-0.29508998359999999</v>
       </c>
       <c r="N15" s="4">
-        <v>-0.37792358760623901</v>
+        <v>-0.32775546849999998</v>
       </c>
       <c r="O15" s="4">
-        <v>-0.38759988127086309</v>
+        <v>-0.32771818409999998</v>
       </c>
       <c r="P15" s="4">
-        <v>-0.36132755199540101</v>
+        <v>-0.32725808360000003</v>
       </c>
       <c r="Q15" s="4">
-        <v>-0.37335515417665699</v>
+        <v>-0.32795720229999997</v>
       </c>
       <c r="R15" s="4">
-        <v>-0.31262835196880601</v>
+        <v>-0.32785511909999898</v>
       </c>
       <c r="S15" s="4">
-        <v>-0.36857917375828403</v>
+        <v>-0.342626737499999</v>
       </c>
       <c r="T15" s="4">
-        <v>-0.29009013615355</v>
+        <v>-0.34198419730000101</v>
       </c>
       <c r="U15" s="4">
-        <v>-0.33518804786981399</v>
+        <v>-0.342547157800001</v>
       </c>
       <c r="V15" s="4">
-        <v>-0.399988360089993</v>
+        <v>-0.34320179969999998</v>
       </c>
       <c r="W15" s="4">
-        <v>-0.31988691783600903</v>
+        <v>-0.34296992100000101</v>
       </c>
       <c r="X15" s="4">
-        <v>-0.31755958479959595</v>
+        <v>-0.42800970090000101</v>
       </c>
       <c r="Y15" s="4">
-        <v>-0.31369644998465401</v>
+        <v>-0.42809877999999901</v>
       </c>
       <c r="Z15" s="4">
-        <v>-0.296045027887887</v>
+        <v>-0.42900656040000001</v>
       </c>
       <c r="AA15" s="4">
-        <v>-0.30862722177435603</v>
-      </c>
-      <c r="AB15" s="4">
-        <v>-0.309062138068257</v>
-      </c>
-      <c r="AC15">
-        <v>-0.29693685476449</v>
-      </c>
-      <c r="AD15">
-        <v>-0.27505925115152602</v>
-      </c>
-      <c r="AE15">
-        <v>-0.24473760610362399</v>
-      </c>
-      <c r="AF15">
-        <v>-0.24656475954628296</v>
-      </c>
-      <c r="AG15">
-        <v>-0.26476597050030798</v>
-      </c>
-      <c r="AH15">
-        <v>-0.22245570919959301</v>
-      </c>
-      <c r="AI15">
-        <v>-0.22419899523269299</v>
-      </c>
-      <c r="AJ15">
-        <v>-0.21516157963982299</v>
-      </c>
+        <v>-0.42908028699999901</v>
+      </c>
+      <c r="AB15" s="4"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="9"/>
@@ -2123,7 +2098,7 @@
   </sheetPr>
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>